<commit_message>
test: Junit test problems: because of duplicate cards. Problems fixed
</commit_message>
<xml_diff>
--- a/v2CorrectionGridBJAssignment.xlsx
+++ b/v2CorrectionGridBJAssignment.xlsx
@@ -972,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2011,7 +2011,7 @@
         <v>35</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="C62" s="6"/>
       <c r="D62">

</xml_diff>